<commit_message>
node voltages 1st iteration
</commit_message>
<xml_diff>
--- a/new Data File .xlsx
+++ b/new Data File .xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -430,6 +430,9 @@
       <c r="I1" t="str">
         <v>ii</v>
       </c>
+      <c r="J1" t="str">
+        <v>v_1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -457,7 +460,10 @@
         <v>11</v>
       </c>
       <c r="I2">
-        <v>23</v>
+        <v>-23</v>
+      </c>
+      <c r="J2" t="str">
+        <v>909.0929545431534∠0.0002494634968685872</v>
       </c>
     </row>
     <row r="3">
@@ -486,7 +492,10 @@
         <v>10</v>
       </c>
       <c r="I3">
-        <v>19</v>
+        <v>-19</v>
+      </c>
+      <c r="J3" t="str">
+        <v>861.0836196328438∠0.00024311240502962285</v>
       </c>
     </row>
     <row r="4">
@@ -515,7 +524,10 @@
         <v>5</v>
       </c>
       <c r="I4">
-        <v>11</v>
+        <v>-11</v>
+      </c>
+      <c r="J4" t="str">
+        <v>802.3895562630411∠0.0005436034131171138</v>
       </c>
     </row>
     <row r="5">
@@ -544,7 +556,10 @@
         <v>2</v>
       </c>
       <c r="I5">
-        <v>7</v>
+        <v>-7</v>
+      </c>
+      <c r="J5" t="str">
+        <v>797.1030359997383∠0.0006786000893114781</v>
       </c>
     </row>
     <row r="6">
@@ -573,12 +588,15 @@
         <v>3</v>
       </c>
       <c r="I6">
-        <v>4</v>
+        <v>-4</v>
+      </c>
+      <c r="J6" t="str">
+        <v>787.0108321999132∠0.0009269517133794074</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>